<commit_message>
Fix: always define cost_breakdown
</commit_message>
<xml_diff>
--- a/dme_dashboard/Operations Final X.xlsx
+++ b/dme_dashboard/Operations Final X.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacksonbogen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacksonbogen/dme_dashboard/dme_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F17783-D798-E545-80E4-B561C3BB2B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F749431-B9A2-374B-9061-FD256974F62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="12640" windowHeight="16260" xr2:uid="{64CC3F8C-9189-8D45-BA8A-5A4D0BC92494}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="12640" windowHeight="16260" firstSheet="1" activeTab="2" xr2:uid="{64CC3F8C-9189-8D45-BA8A-5A4D0BC92494}"/>
   </bookViews>
   <sheets>
     <sheet name="SupplyClean" sheetId="7" r:id="rId1"/>
@@ -740,6 +740,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -752,16 +754,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -770,14 +763,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,7 +1114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7226AF2-9218-E640-9494-3B99FE2F5BD1}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -1296,22 +1296,22 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
@@ -1328,13 +1328,13 @@
       <c r="H13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.2">
       <c r="F14" s="2" t="s">
@@ -1403,13 +1403,13 @@
       </c>
     </row>
     <row r="21" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
     </row>
     <row r="22" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F22" s="5" t="s">
@@ -1488,26 +1488,26 @@
       </c>
     </row>
     <row r="31" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F31" s="25" t="s">
+      <c r="F31" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
     </row>
     <row r="32" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
     </row>
     <row r="33" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F33" s="3" t="s">
@@ -1671,11 +1671,11 @@
       </c>
     </row>
     <row r="41" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
     </row>
     <row r="42" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F42" s="3" t="s">
@@ -1755,11 +1755,11 @@
       </c>
     </row>
     <row r="49" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
     </row>
     <row r="50" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F50" s="3" t="s">
@@ -1789,10 +1789,10 @@
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F53" s="16" t="s">
+      <c r="F53" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="G53" s="17"/>
+      <c r="G53" s="19"/>
     </row>
     <row r="54" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F54" s="3" t="s">
@@ -1908,18 +1908,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="3" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D4" s="3" t="s">
@@ -2279,11 +2279,11 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
       <c r="H11" s="2" t="s">
         <v>98</v>
       </c>
@@ -2408,11 +2408,11 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="2" t="s">
         <v>94</v>
       </c>
@@ -2590,18 +2590,18 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="2:23" ht="22" x14ac:dyDescent="0.3">
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
       <c r="J6" s="7"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
@@ -2629,10 +2629,10 @@
         <v>14</v>
       </c>
       <c r="J7" s="7"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
@@ -2660,10 +2660,10 @@
         <v>78</v>
       </c>
       <c r="J8" s="7"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
@@ -2775,13 +2775,13 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="22"/>
+      <c r="W12" s="22"/>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
@@ -2850,14 +2850,14 @@
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="2:23" ht="22" x14ac:dyDescent="0.3">
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
       <c r="J16" s="7"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2964,13 +2964,13 @@
         <v>136</v>
       </c>
       <c r="J20" s="7"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
@@ -3145,13 +3145,13 @@
         <v>32</v>
       </c>
       <c r="J30" s="7"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
@@ -3173,13 +3173,13 @@
         <v>37</v>
       </c>
       <c r="J31" s="7"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21"/>
-      <c r="S31" s="21"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="25"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
+      <c r="S31" s="25"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
@@ -3328,9 +3328,9 @@
         <v>85</v>
       </c>
       <c r="J40" s="7"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
@@ -3385,9 +3385,9 @@
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.2">
       <c r="J48" s="7"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
     </row>
     <row r="49" spans="10:15" x14ac:dyDescent="0.2">
       <c r="J49" s="7"/>
@@ -3409,8 +3409,8 @@
     </row>
     <row r="52" spans="10:15" x14ac:dyDescent="0.2">
       <c r="J52" s="7"/>
-      <c r="M52" s="16"/>
-      <c r="N52" s="17"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="19"/>
     </row>
     <row r="53" spans="10:15" x14ac:dyDescent="0.2">
       <c r="J53" s="7"/>
@@ -3934,7 +3934,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4088,8 +4088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00E9E3B-4650-0149-84DF-E28F38EC3609}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4112,13 +4112,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="14">
         <v>4.7</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="14">
         <v>23.4</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4129,13 +4129,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="14">
         <v>21.7</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="14">
         <v>17.600000000000001</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -4146,13 +4146,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="14">
         <v>7.4</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="14">
         <v>24.3</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -4163,13 +4163,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="14">
         <v>13.7</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="14">
         <v>9.8000000000000007</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -4180,13 +4180,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="14">
         <v>6.1</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="14">
         <v>14.1</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -4197,13 +4197,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="14">
         <v>6</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="14">
         <v>31.6</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -4223,41 +4223,41 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="14" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="14">
         <v>19.399999999999999</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="14">
         <v>33.4</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="14" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4288,7 +4288,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
@@ -4299,7 +4299,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
@@ -4310,7 +4310,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
@@ -4321,7 +4321,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
@@ -4332,7 +4332,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2">
@@ -4343,7 +4343,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
@@ -4424,42 +4424,42 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="15">
         <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="15">
         <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="15">
         <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="15">
         <v>0.7</v>
       </c>
     </row>

</xml_diff>